<commit_message>
// ??? it works ??? why?
</commit_message>
<xml_diff>
--- a/docs/pipeflow.xlsx
+++ b/docs/pipeflow.xlsx
@@ -349,16 +349,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>273597</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>88681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>409227</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>18845</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>616149</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -375,8 +375,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4333875" y="3143250"/>
-          <a:ext cx="2780952" cy="1638095"/>
+          <a:off x="3508813" y="2075793"/>
+          <a:ext cx="2930724" cy="1549414"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -653,11 +653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="3" spans="2:17">
       <c r="C3" t="s">
@@ -1042,105 +1042,121 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.99</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="1">
         <f>C19-C21</f>
-        <v>-0.39</v>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="L21">
+        <f>PI()*0.3^2</f>
+        <v>0.28274333882308139</v>
       </c>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2" t="e">
-        <f>2*ACOS((C20-D21)/C20)</f>
-        <v>#NUM!</v>
+      <c r="C22" s="2">
+        <f>2*ACOS((C20-C21)/C20)</f>
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="L22">
+        <f>2*L21</f>
+        <v>0.56548667764616278</v>
       </c>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="C23" t="e">
+      <c r="C23">
         <f>PI()*C20^2-(C20^2)*(C22-SIN(C22))/2</f>
-        <v>#NUM!</v>
+        <v>3.0974820801117908E-2</v>
+      </c>
+      <c r="L23">
+        <f>L22/PI()</f>
+        <v>0.18</v>
       </c>
     </row>
     <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" t="e">
+      <c r="C24">
         <f>2*PI()*C20-C20*C22</f>
-        <v>#NUM!</v>
+        <v>0.50464120234075804</v>
+      </c>
+      <c r="L24">
+        <f>SQRT(L23)</f>
+        <v>0.42426406871192851</v>
       </c>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>1</v>
       </c>
-      <c r="C25" t="e">
+      <c r="C25">
         <f>C23/C24</f>
-        <v>#NUM!</v>
+        <v>6.1379888636604464E-2</v>
       </c>
     </row>
     <row r="26" spans="2:17">
-      <c r="D26" s="3" t="e">
+      <c r="D26" s="3">
         <f>2*PI()-D27</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E26" s="3" t="e">
+        <v>4.3682243048167129</v>
+      </c>
+      <c r="E26" s="3">
         <f t="shared" ref="E26:Q26" si="4">2*PI()-E27</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F26" s="3" t="e">
+        <v>4.5815275743891402</v>
+      </c>
+      <c r="F26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G26" s="3" t="e">
+        <v>4.6008807377552472</v>
+      </c>
+      <c r="G26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H26" s="3" t="e">
+        <v>4.6010479535392896</v>
+      </c>
+      <c r="H26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="I26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="J26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="K26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="L26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="M26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="N26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="O26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="P26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q26" s="3" t="e">
+        <v>4.6010479660437262</v>
+      </c>
+      <c r="Q26" s="3">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
+        <v>4.6010479660437262</v>
       </c>
     </row>
     <row r="27" spans="2:17">
@@ -1151,126 +1167,126 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="D27" t="e">
+      <c r="D27">
         <f>C27-C30/C29</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E27" t="e">
+        <v>1.9149610023628734</v>
+      </c>
+      <c r="E27">
         <f>D27-D30/D29</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F27" t="e">
+        <v>1.7016577327904463</v>
+      </c>
+      <c r="F27">
         <f t="shared" ref="F27:Q27" si="5">E27-E30/E29</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G27" t="e">
+        <v>1.6823045694243395</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H27" t="e">
+        <v>1.6821373536402964</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="O27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q27" t="e">
+        <v>1.6821373411358602</v>
+      </c>
+      <c r="Q27">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
+        <v>1.6821373411358602</v>
       </c>
     </row>
     <row r="28" spans="2:17">
       <c r="B28" t="s">
         <v>11</v>
       </c>
-      <c r="C28" t="e">
+      <c r="C28">
         <f>2*C23/(C20^2)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="D28">
         <f>C28</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="E28">
         <f t="shared" ref="E28:Q28" si="6">D28</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="G28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="N28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="O28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q28" t="e">
+        <v>0.6883293511359535</v>
+      </c>
+      <c r="Q28">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>0.6883293511359535</v>
       </c>
     </row>
     <row r="29" spans="2:17">
@@ -1281,144 +1297,144 @@
         <f>1-COS(C27)</f>
         <v>2</v>
       </c>
-      <c r="D29" t="e">
+      <c r="D29">
         <f>1-COS(D27)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E29" t="e">
+        <v>1.3374104560300535</v>
+      </c>
+      <c r="E29">
         <f>1-COS(E27)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F29" t="e">
+        <v>1.1304882317786891</v>
+      </c>
+      <c r="F29">
         <f t="shared" ref="F29:Q29" si="7">1-COS(F27)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G29" t="e">
+        <v>1.111277302365953</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H29" t="e">
+        <v>1.1111111235381195</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="N29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="O29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q29" t="e">
+        <v>1.1111111111111107</v>
+      </c>
+      <c r="Q29">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>1.1111111111111107</v>
       </c>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C30" t="e">
+      <c r="C30">
         <f>-SIN(C27)+C27-C28</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D30" t="e">
+        <v>2.4532633024538395</v>
+      </c>
+      <c r="D30">
         <f>-SIN(D27)+D27-D28</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E30" t="e">
+        <v>0.28527402303156102</v>
+      </c>
+      <c r="E30">
         <f>-SIN(E27)+E27-E28</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F30" t="e">
+        <v>2.1878523433074171E-2</v>
+      </c>
+      <c r="F30">
         <f t="shared" ref="F30:Q30" si="8">-SIN(F27)+F27-F28</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G30" t="e">
+        <v>1.8582310540449232E-4</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H30" t="e">
+        <v>1.3893818207044717E-8</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I30" t="e">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J30" t="e">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K30" t="e">
+        <v>0</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L30" t="e">
+        <v>0</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M30" t="e">
+        <v>0</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N30" t="e">
+        <v>0</v>
+      </c>
+      <c r="N30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O30" t="e">
+        <v>0</v>
+      </c>
+      <c r="O30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P30" t="e">
+        <v>0</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q30" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q30">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:17">
       <c r="G31" t="s">
         <v>14</v>
       </c>
-      <c r="H31" t="e">
+      <c r="H31">
         <f>C20-COS(H27/2)*C20</f>
-        <v>#NUM!</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="32" spans="2:17">
       <c r="P32" t="s">
         <v>3</v>
       </c>
-      <c r="Q32" t="e">
+      <c r="Q32">
         <f>C20-COS(Q27/2)*C20</f>
-        <v>#NUM!</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="33" spans="3:3">

</xml_diff>